<commit_message>
Kosztorys + zmiana seat_capacity
</commit_message>
<xml_diff>
--- a/bazy_projekt.xlsx
+++ b/bazy_projekt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4e11ade123241e18/Dokumenty/Studia/semestr6/Bazy danych/projekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="205" documentId="8_{8CA045E8-E3E7-483E-A8C8-8CF5162D7C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A61946A-F2A9-4A44-814C-E29B30451CAE}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="8_{8CA045E8-E3E7-483E-A8C8-8CF5162D7C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67FE9562-EF12-48AF-B0E5-EEE9FC78568B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{71011B89-52BF-4F10-A8D7-10F7B7092A5E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Wycieczka</t>
   </si>
@@ -92,25 +92,22 @@
     <t>przewodnik</t>
   </si>
   <si>
-    <t>liczba lotów</t>
-  </si>
-  <si>
-    <t>liczba pasażerów</t>
-  </si>
-  <si>
-    <t>LOTY</t>
-  </si>
-  <si>
     <t>Przewidywane zyski firmy (okres 2 letni)</t>
   </si>
   <si>
-    <t>PENSJE (miesięczne)</t>
-  </si>
-  <si>
     <t>ZYSK</t>
   </si>
   <si>
     <t>cały koszt działalności</t>
+  </si>
+  <si>
+    <t>PENSJE (miesięczne, bez bonusu)</t>
+  </si>
+  <si>
+    <t>liczba płatności</t>
+  </si>
+  <si>
+    <t>LOTY (przewidywana liczba płatności)</t>
   </si>
 </sst>
 </file>
@@ -196,7 +193,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -219,25 +216,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -581,15 +618,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BA5CA1C-9842-4763-9DA4-DEB0FD49DC26}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7265625" customWidth="1"/>
     <col min="4" max="4" width="18.90625" customWidth="1"/>
     <col min="5" max="5" width="7.26953125" customWidth="1"/>
@@ -599,12 +637,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="9">
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="10">
         <v>200</v>
       </c>
     </row>
@@ -658,7 +696,7 @@
         <f>D4*C4+E4+F4</f>
         <v>4500</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="7">
         <f>AVERAGE(G4:G10)</f>
         <v>3364.2857142857142</v>
       </c>
@@ -684,10 +722,10 @@
         <v>12000</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" ref="G5:G10" si="1">D5*C5+E5+F5</f>
+        <f>D5*C5+E5+F5</f>
         <v>3200</v>
       </c>
-      <c r="H5" s="5"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -710,10 +748,10 @@
         <v>8000</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G6:G10" si="1">D6*C6+E6+F6</f>
         <v>4000</v>
       </c>
-      <c r="H6" s="5"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
@@ -739,7 +777,7 @@
         <f t="shared" si="1"/>
         <v>3000</v>
       </c>
-      <c r="H7" s="5"/>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -765,7 +803,7 @@
         <f t="shared" si="1"/>
         <v>3100</v>
       </c>
-      <c r="H8" s="5"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -791,7 +829,7 @@
         <f>D9*C9+E9+F9</f>
         <v>2650</v>
       </c>
-      <c r="H9" s="5"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
@@ -817,70 +855,62 @@
         <f t="shared" si="1"/>
         <v>3100</v>
       </c>
-      <c r="H10" s="5"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="A14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="6">
         <v>-9000</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="6">
         <v>-6000</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="8">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="8">
-        <f>3*2*12*(B17+B18)+B21*B22*H4</f>
-        <v>7667142.8571428563</v>
+      <c r="B24" s="3">
+        <f>3*2*12*(B17+B18)+B21*H4</f>
+        <v>-212014.28571428568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>